<commit_message>
Set up Results screen, Feedback screens, and fixed bugs
</commit_message>
<xml_diff>
--- a/resources/PWS_By_Municipality.xlsx
+++ b/resources/PWS_By_Municipality.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Desktop\Code\Local Projects\GSSTeam12Project\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8B3B08-4385-4295-9535-82816EFD4E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C68E5E3-ADB7-4C7B-BF8C-D2D08FCEF2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5081,6 +5081,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C874F097-43B4-4C1F-BA7F-1FD7FFF5026A}" name="Table1" displayName="Table1" ref="A1:F1048576" totalsRowShown="0">
+  <autoFilter ref="A1:F1048576" xr:uid="{C874F097-43B4-4C1F-BA7F-1FD7FFF5026A}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{07B692B0-670F-4101-8287-5B5D2B7016CF}" name="PWSID"/>
+    <tableColumn id="2" xr3:uid="{5A33A6E5-31F7-4392-BD90-CD238A886B52}" name="Water System Name"/>
+    <tableColumn id="3" xr3:uid="{FC795FDB-2EEB-4064-B1B7-40C39E1C33AB}" name="System Type"/>
+    <tableColumn id="4" xr3:uid="{35F50A8D-4316-4161-BA5D-78178843D6A5}" name="Municipality"/>
+    <tableColumn id="5" xr3:uid="{108D2F6F-E0FB-40BE-B9D1-B68390983892}" name="County"/>
+    <tableColumn id="6" xr3:uid="{B70662D8-FC22-4E28-9C13-3784B21E1C74}" name="Population"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5377,7 +5392,7 @@
   <dimension ref="A1:F996"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -25295,5 +25310,8 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>